<commit_message>
updates from last run aug 18
</commit_message>
<xml_diff>
--- a/param_files/birth_rate_gen/HIV_prev_birth_rate.xlsx
+++ b/param_files/birth_rate_gen/HIV_prev_birth_rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/param_files/birth_rate_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70E24F2-501F-2845-BEA4-7FEACA4D6777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D8DC98-3836-A745-8498-899190E59C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="20660" xr2:uid="{93EE70CD-6823-4B43-A470-F3A81EB6857D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="20560" xr2:uid="{93EE70CD-6823-4B43-A470-F3A81EB6857D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -921,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AD8033-F70E-4E7C-9BDE-258BA5A81ADC}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <f t="shared" ref="A42:A79" si="2">A3</f>
+        <f t="shared" ref="A42:A78" si="2">A3</f>
         <v>1981</v>
       </c>
       <c r="B42" s="2">
@@ -2205,19 +2205,337 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="2">
-        <f t="shared" si="2"/>
+      <c r="A79" s="6">
         <v>2018</v>
       </c>
       <c r="B79" s="2">
         <v>2</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="6">
         <v>7.8438382554176496</v>
       </c>
       <c r="D79" s="7">
-        <f t="shared" si="3"/>
+        <f>C79*0.01</f>
         <v>7.8438382554176497E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="6">
+        <f>A79+1</f>
+        <v>2019</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2</v>
+      </c>
+      <c r="C80" s="6">
+        <v>7.4114267673995897</v>
+      </c>
+      <c r="D80" s="7">
+        <f t="shared" ref="D80:D99" si="4">C80*0.01</f>
+        <v>7.4114267673995898E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <f t="shared" ref="A81:A89" si="5">A80+1</f>
+        <v>2020</v>
+      </c>
+      <c r="B81" s="2">
+        <v>2</v>
+      </c>
+      <c r="C81" s="6">
+        <v>7.0116812689368802</v>
+      </c>
+      <c r="D81" s="7">
+        <f t="shared" si="4"/>
+        <v>7.0116812689368799E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <f t="shared" si="5"/>
+        <v>2021</v>
+      </c>
+      <c r="B82" s="2">
+        <v>2</v>
+      </c>
+      <c r="C82" s="6">
+        <v>6.7063135897258102</v>
+      </c>
+      <c r="D82" s="7">
+        <f t="shared" si="4"/>
+        <v>6.7063135897258097E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <f t="shared" si="5"/>
+        <v>2022</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2</v>
+      </c>
+      <c r="C83" s="6">
+        <v>6.3751951909781202</v>
+      </c>
+      <c r="D83" s="7">
+        <f t="shared" si="4"/>
+        <v>6.3751951909781196E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="6">
+        <f t="shared" si="5"/>
+        <v>2023</v>
+      </c>
+      <c r="B84" s="2">
+        <v>2</v>
+      </c>
+      <c r="C84" s="6">
+        <v>6.0822652358209801</v>
+      </c>
+      <c r="D84" s="7">
+        <f t="shared" si="4"/>
+        <v>6.08226523582098E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <f t="shared" si="5"/>
+        <v>2024</v>
+      </c>
+      <c r="B85" s="2">
+        <v>2</v>
+      </c>
+      <c r="C85" s="6">
+        <v>5.8256009971171396</v>
+      </c>
+      <c r="D85" s="7">
+        <f t="shared" si="4"/>
+        <v>5.8256009971171398E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="6">
+        <f t="shared" si="5"/>
+        <v>2025</v>
+      </c>
+      <c r="B86" s="2">
+        <v>2</v>
+      </c>
+      <c r="C86" s="6">
+        <v>5.6024729674422904</v>
+      </c>
+      <c r="D86" s="7">
+        <f t="shared" si="4"/>
+        <v>5.6024729674422902E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <f t="shared" si="5"/>
+        <v>2026</v>
+      </c>
+      <c r="B87" s="2">
+        <v>2</v>
+      </c>
+      <c r="C87" s="6">
+        <v>5.4096632124577697</v>
+      </c>
+      <c r="D87" s="7">
+        <f t="shared" si="4"/>
+        <v>5.4096632124577701E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="6">
+        <f t="shared" si="5"/>
+        <v>2027</v>
+      </c>
+      <c r="B88" s="2">
+        <v>2</v>
+      </c>
+      <c r="C88" s="6">
+        <v>5.2437770976533002</v>
+      </c>
+      <c r="D88" s="7">
+        <f t="shared" si="4"/>
+        <v>5.2437770976533002E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
+        <f t="shared" si="5"/>
+        <v>2028</v>
+      </c>
+      <c r="B89" s="2">
+        <v>2</v>
+      </c>
+      <c r="C89" s="6">
+        <v>5.1014583304981604</v>
+      </c>
+      <c r="D89" s="7">
+        <f t="shared" si="4"/>
+        <v>5.1014583304981605E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>2019</v>
+      </c>
+      <c r="B90" s="2">
+        <v>1</v>
+      </c>
+      <c r="C90" s="6">
+        <v>0.73832369161317501</v>
+      </c>
+      <c r="D90" s="7">
+        <f>C90*0.01</f>
+        <v>7.3832369161317499E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
+        <f t="shared" ref="A91:A99" si="6">A90+1</f>
+        <v>2020</v>
+      </c>
+      <c r="B91" s="2">
+        <v>1</v>
+      </c>
+      <c r="C91" s="6">
+        <v>0.66802340000248694</v>
+      </c>
+      <c r="D91" s="7">
+        <f t="shared" si="4"/>
+        <v>6.6802340000248692E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
+        <f t="shared" si="6"/>
+        <v>2021</v>
+      </c>
+      <c r="B92" s="2">
+        <v>1</v>
+      </c>
+      <c r="C92" s="6">
+        <v>0.61709766979277303</v>
+      </c>
+      <c r="D92" s="7">
+        <f t="shared" si="4"/>
+        <v>6.1709766979277303E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <f t="shared" si="6"/>
+        <v>2022</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1</v>
+      </c>
+      <c r="C93" s="6">
+        <v>0.56648689358034099</v>
+      </c>
+      <c r="D93" s="7">
+        <f t="shared" si="4"/>
+        <v>5.6648689358034096E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
+        <f t="shared" si="6"/>
+        <v>2023</v>
+      </c>
+      <c r="B94" s="2">
+        <v>1</v>
+      </c>
+      <c r="C94" s="6">
+        <v>0.52555582168721704</v>
+      </c>
+      <c r="D94" s="7">
+        <f t="shared" si="4"/>
+        <v>5.2555582168721708E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
+        <f t="shared" si="6"/>
+        <v>2024</v>
+      </c>
+      <c r="B95" s="2">
+        <v>1</v>
+      </c>
+      <c r="C95" s="6">
+        <v>0.49261008571194198</v>
+      </c>
+      <c r="D95" s="7">
+        <f t="shared" si="4"/>
+        <v>4.9261008571194198E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
+        <f t="shared" si="6"/>
+        <v>2025</v>
+      </c>
+      <c r="B96" s="2">
+        <v>1</v>
+      </c>
+      <c r="C96" s="6">
+        <v>0.46616638883279099</v>
+      </c>
+      <c r="D96" s="7">
+        <f t="shared" si="4"/>
+        <v>4.6616638883279103E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <f t="shared" si="6"/>
+        <v>2026</v>
+      </c>
+      <c r="B97" s="2">
+        <v>1</v>
+      </c>
+      <c r="C97" s="6">
+        <v>0.44497048215463603</v>
+      </c>
+      <c r="D97" s="7">
+        <f t="shared" si="4"/>
+        <v>4.4497048215463601E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
+        <f t="shared" si="6"/>
+        <v>2027</v>
+      </c>
+      <c r="B98" s="2">
+        <v>1</v>
+      </c>
+      <c r="C98" s="6">
+        <v>0.42798405610575402</v>
+      </c>
+      <c r="D98" s="7">
+        <f t="shared" si="4"/>
+        <v>4.2798405610575399E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <f t="shared" si="6"/>
+        <v>2028</v>
+      </c>
+      <c r="B99" s="2">
+        <v>1</v>
+      </c>
+      <c r="C99" s="6">
+        <v>0.41435498869028597</v>
+      </c>
+      <c r="D99" s="7">
+        <f t="shared" si="4"/>
+        <v>4.14354988690286E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>